<commit_message>
trying to do some automatization
</commit_message>
<xml_diff>
--- a/public/dataTable.xlsx
+++ b/public/dataTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kotawski\Coding\estimationCenter\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC03BCC5-2517-4276-9F39-CF95F45CA4F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0880165A-FF22-4B4B-ADE1-39FD3058EF6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F53F1143-5114-4282-8AF3-5DBDBA634C13}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F53F1143-5114-4282-8AF3-5DBDBA634C13}"/>
   </bookViews>
   <sheets>
     <sheet name="EC" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -206,15 +207,6 @@
     <t>parklifty</t>
   </si>
   <si>
-    <t>Romanowicza</t>
-  </si>
-  <si>
-    <t>Kraków</t>
-  </si>
-  <si>
-    <t>Finished</t>
-  </si>
-  <si>
     <t>powierzchnia zabudowy nadziemia</t>
   </si>
   <si>
@@ -222,6 +214,15 @@
   </si>
   <si>
     <t>zieleń</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Bardzka</t>
+  </si>
+  <si>
+    <t>Wrocław</t>
   </si>
 </sst>
 </file>
@@ -295,7 +296,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -311,6 +312,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Dziesiętny" xfId="2" builtinId="3"/>
@@ -342,8 +344,10 @@
       <sheetName val="Bardzka - wycinki"/>
       <sheetName val="Bardzka - ektryczna"/>
       <sheetName val="Bardzka - PORR GW"/>
+      <sheetName val="Bardzka  - CONTRACT SIGNEDv2"/>
       <sheetName val="Bardzka  - CONTRACT SIGNED"/>
       <sheetName val="Pohoskiego - kody I"/>
+      <sheetName val="Pohoskiego - contract signedv2"/>
       <sheetName val="Pohoskiego - contract signed"/>
       <sheetName val="Pohoskiego - zabezpieczenie wyk"/>
       <sheetName val="Pohoskiego SS"/>
@@ -387,7 +391,9 @@
       <sheetName val="Stocznia Remediacja A1"/>
       <sheetName val="Stocznia Remediacja"/>
       <sheetName val="Stocznia - ogrodzenie"/>
+      <sheetName val="Stocznia - contract signedv2"/>
       <sheetName val="Stocznia - contract signed"/>
+      <sheetName val="Romanowicza - contract signedv2"/>
       <sheetName val="Romanowicza - contract signed"/>
       <sheetName val="Stocznia - Keller"/>
       <sheetName val="Brnenska - zasilanie placu budo"/>
@@ -447,8 +453,6 @@
       <sheetName val="Jana Pawła - TES (4)"/>
       <sheetName val="Jana Pawła - Oferta stan zero"/>
       <sheetName val="Jana Pawła - Oferta nadziemie"/>
-      <sheetName val="R4R"/>
-      <sheetName val="EC"/>
       <sheetName val="Jana Pawła - deweloperski (4)"/>
       <sheetName val="Jana Pawła - Drogi i Zieleń"/>
       <sheetName val="Jana Pawła - Instalacje san"/>
@@ -471,9 +475,19 @@
       <sheetName val="Zielony Trojkat - budget"/>
       <sheetName val="Curtis - Kody I"/>
       <sheetName val="Opaczewska - Kody I"/>
+      <sheetName val="Brnenska - wyk2"/>
+      <sheetName val="Brnenska - wyk"/>
+      <sheetName val="Brnenska - contract signedv2"/>
       <sheetName val="Brnenska - contract signed"/>
+      <sheetName val="R4R"/>
       <sheetName val="Wykończenie budowlane"/>
       <sheetName val="Stan surowy"/>
+      <sheetName val="EC - ROMANOWICZA"/>
+      <sheetName val="EC - STOCZNIA"/>
+      <sheetName val="EC - BRNEŃSKA"/>
+      <sheetName val="EC - POHOSKIEGO"/>
+      <sheetName val="EC - BARDZKA"/>
+      <sheetName val="EC - JANA PAWŁA"/>
       <sheetName val="Opaczewska - keller"/>
       <sheetName val="Bardzka - Kody I"/>
       <sheetName val="udział SS do N03 - umowy"/>
@@ -621,173 +635,7 @@
       <sheetData sheetId="107"/>
       <sheetData sheetId="108"/>
       <sheetData sheetId="109"/>
-      <sheetData sheetId="110">
-        <row r="4">
-          <cell r="E4">
-            <v>13189</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="E5">
-            <v>5849</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="E6">
-            <v>9883</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="E9">
-            <v>9380.0700000000015</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="E10">
-            <v>36380.17</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="E11">
-            <v>27839</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="E12">
-            <v>1692</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="E13">
-            <v>29531</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="E15">
-            <v>324</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="E16">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="E17">
-            <v>873</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="E26">
-            <v>1100000</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="E37">
-            <v>167716386.99774998</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="E39">
-            <v>1915808.6847999992</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="E40">
-            <v>4414079</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="E44">
-            <v>8475964.5531971008</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="E45">
-            <v>8992347.2480222024</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="E46">
-            <v>32274693.513980698</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="E47">
-            <v>21488112.304190762</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="E48">
-            <v>6543614.858957001</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="E49">
-            <v>3846666.5490708007</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="E50">
-            <v>26541918.295966305</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="E52">
-            <v>1485160</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="E54">
-            <v>17174560.004198376</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="E55">
-            <v>7153414.9939294979</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="E57">
-            <v>10494992.387217235</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="E58">
-            <v>8154123.2635999983</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="E59">
-            <v>1560231.9930200002</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="E60">
-            <v>233553</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="E61">
-            <v>990810</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="E62">
-            <v>1921850.3476</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="E63">
-            <v>308215</v>
-          </cell>
-        </row>
-        <row r="65">
-          <cell r="E65">
-            <v>3746271</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="110"/>
       <sheetData sheetId="111"/>
       <sheetData sheetId="112"/>
       <sheetData sheetId="113"/>
@@ -817,7 +665,188 @@
       <sheetData sheetId="137"/>
       <sheetData sheetId="138"/>
       <sheetData sheetId="139"/>
-      <sheetData sheetId="140"/>
+      <sheetData sheetId="140">
+        <row r="4">
+          <cell r="M4">
+            <v>8627</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="M5">
+            <v>3614</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="M6">
+            <v>6005</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="M9">
+            <v>5686.89</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="M10">
+            <v>28310.68</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="M11">
+            <v>20099</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="M12">
+            <v>982</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="M13">
+            <v>21081</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="M15">
+            <v>261</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="M16">
+            <v>52</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="M17">
+            <v>620</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="M26">
+            <v>2209809.9493262982</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="M37">
+            <v>126474582.04596475</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="M39">
+            <v>1696355.7778052683</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="M40">
+            <v>765180.12408676615</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="M44">
+            <v>7958639.9526595371</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="M45">
+            <v>4685708.039493002</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="M46">
+            <v>27584187.476333722</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="M47">
+            <v>13930473.462220209</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="M48">
+            <v>3051304.4601880657</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="M49">
+            <v>1725842.7947463281</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="M50">
+            <v>16924122.340030454</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="M52">
+            <v>1450919.5928848851</v>
+          </cell>
+        </row>
+        <row r="53">
+          <cell r="M53">
+            <v>1525039.6573558222</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="M54">
+            <v>11478928.094861932</v>
+          </cell>
+        </row>
+        <row r="55">
+          <cell r="M55">
+            <v>6017422.8093521548</v>
+          </cell>
+        </row>
+        <row r="56">
+          <cell r="M56">
+            <v>35515.288902255757</v>
+          </cell>
+        </row>
+        <row r="57">
+          <cell r="M57">
+            <v>10454941.525389537</v>
+          </cell>
+        </row>
+        <row r="58">
+          <cell r="M58">
+            <v>5951138.570044524</v>
+          </cell>
+        </row>
+        <row r="59">
+          <cell r="M59">
+            <v>884136.18510875478</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="M60">
+            <v>700230.30960916413</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="M61">
+            <v>178623.43460676802</v>
+          </cell>
+        </row>
+        <row r="62">
+          <cell r="M62">
+            <v>651387.58731839038</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="M63">
+            <v>6022436.9343661135</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="M64">
+            <v>983112.62860110216</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="M65">
+            <v>1818935</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="141"/>
       <sheetData sheetId="142"/>
       <sheetData sheetId="143"/>
@@ -849,6 +878,98 @@
       <sheetData sheetId="169"/>
       <sheetData sheetId="170"/>
       <sheetData sheetId="171"/>
+      <sheetData sheetId="172"/>
+      <sheetData sheetId="173"/>
+      <sheetData sheetId="174"/>
+      <sheetData sheetId="175"/>
+      <sheetData sheetId="176"/>
+      <sheetData sheetId="177"/>
+      <sheetData sheetId="178"/>
+      <sheetData sheetId="179"/>
+      <sheetData sheetId="180"/>
+      <sheetData sheetId="181"/>
+      <sheetData sheetId="182"/>
+      <sheetData sheetId="183"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="PRZEZENTACJA_ETAPY"/>
+      <sheetName val="WZÓR ECHO"/>
+      <sheetName val="Analiza cz1"/>
+      <sheetName val="Analiza cz2"/>
+      <sheetName val="wykonczenie sanitarne"/>
+      <sheetName val="wykonczenie elektryczne"/>
+      <sheetName val="dane pow 1"/>
+      <sheetName val="szac"/>
+      <sheetName val="dane powierzchniowe"/>
+      <sheetName val="wyk sanitarne"/>
+      <sheetName val="wyk elektryczne"/>
+      <sheetName val="sieci sanitarne "/>
+      <sheetName val="Wycena szacunkowa"/>
+      <sheetName val="Kody I"/>
+      <sheetName val="Szczegóły"/>
+      <sheetName val="Powierzchnie"/>
+      <sheetName val="Koszty budowy"/>
+      <sheetName val="pomocnicza"/>
+      <sheetName val="Opłata przyłączeniowa"/>
+      <sheetName val="Prace przeniesione do GW - E.Ł."/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14">
+        <row r="96">
+          <cell r="BP96">
+            <v>20953.95498000001</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="15">
+        <row r="15">
+          <cell r="BV15">
+            <v>2391</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="BP18">
+            <v>571.49</v>
+          </cell>
+          <cell r="BV18">
+            <v>1377</v>
+          </cell>
+          <cell r="BY18">
+            <v>956.77</v>
+          </cell>
+          <cell r="CA18">
+            <v>1579.1</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1174,12 +1295,13 @@
   <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection sqref="A1:B54"/>
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1187,7 +1309,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1195,10 +1317,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="300" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1211,7 +1333,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1219,8 +1341,8 @@
         <v>4</v>
       </c>
       <c r="B5" s="4">
-        <f>[1]R4R!E37/[1]R4R!E13</f>
-        <v>5679.3331413683918</v>
+        <f>[1]R4R!M37/[1]R4R!M13</f>
+        <v>5999.4583770202908</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1228,26 +1350,26 @@
         <v>9</v>
       </c>
       <c r="B6" s="6">
-        <f>[1]R4R!E4</f>
-        <v>13189</v>
+        <f>[1]R4R!M4</f>
+        <v>8627</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B7" s="6">
-        <f>[1]R4R!E5</f>
-        <v>5849</v>
+        <f>[1]R4R!M5</f>
+        <v>3614</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B8" s="6">
-        <f>[1]R4R!E6</f>
-        <v>9883</v>
+        <f>[1]R4R!M6</f>
+        <v>6005</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1264,7 +1386,7 @@
       </c>
       <c r="B10" s="6">
         <f>B6-B7</f>
-        <v>7340</v>
+        <v>5013</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1272,7 +1394,8 @@
         <v>11</v>
       </c>
       <c r="B11" s="6">
-        <v>10571</v>
+        <f>[2]Powierzchnie!$CA$18+[2]Powierzchnie!$BY$18+[2]Powierzchnie!$BV$18+[2]Powierzchnie!$BV$15</f>
+        <v>6303.87</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1280,7 +1403,8 @@
         <v>12</v>
       </c>
       <c r="B12" s="6">
-        <v>29249.055</v>
+        <f>[2]Szczegóły!$BP$96</f>
+        <v>20953.95498000001</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1289,7 +1413,7 @@
       </c>
       <c r="B13" s="6">
         <f>B14+B15</f>
-        <v>45760.24</v>
+        <v>33997.57</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1297,8 +1421,8 @@
         <v>14</v>
       </c>
       <c r="B14" s="6">
-        <f>[1]R4R!E9</f>
-        <v>9380.0700000000015</v>
+        <f>[1]R4R!M9</f>
+        <v>5686.89</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1306,8 +1430,8 @@
         <v>15</v>
       </c>
       <c r="B15" s="6">
-        <f>[1]R4R!E10</f>
-        <v>36380.17</v>
+        <f>[1]R4R!M10</f>
+        <v>28310.68</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1316,7 +1440,7 @@
       </c>
       <c r="B16" s="6">
         <f>B17+B18</f>
-        <v>29531</v>
+        <v>21081</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1324,8 +1448,8 @@
         <v>17</v>
       </c>
       <c r="B17" s="6">
-        <f>[1]R4R!E11</f>
-        <v>27839</v>
+        <f>[1]R4R!M11</f>
+        <v>20099</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1333,8 +1457,8 @@
         <v>18</v>
       </c>
       <c r="B18" s="6">
-        <f>[1]R4R!E12</f>
-        <v>1692</v>
+        <f>[1]R4R!M12</f>
+        <v>982</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1343,7 +1467,7 @@
       </c>
       <c r="B19" s="6">
         <f>B15-B17-B18</f>
-        <v>6849.1699999999983</v>
+        <v>7229.68</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1351,7 +1475,8 @@
         <v>20</v>
       </c>
       <c r="B20" s="6">
-        <v>735</v>
+        <f>[2]Powierzchnie!$BP$18</f>
+        <v>571.49</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1359,7 +1484,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="6">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1367,8 +1492,8 @@
         <v>49</v>
       </c>
       <c r="B22" s="6">
-        <f>[1]R4R!E15</f>
-        <v>324</v>
+        <f>[1]R4R!M15</f>
+        <v>261</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1376,8 +1501,8 @@
         <v>22</v>
       </c>
       <c r="B23" s="6">
-        <f>[1]R4R!E16</f>
-        <v>0</v>
+        <f>[1]R4R!M16</f>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1385,8 +1510,8 @@
         <v>23</v>
       </c>
       <c r="B24" s="6">
-        <f>[1]R4R!E17</f>
-        <v>873</v>
+        <f>[1]R4R!M17</f>
+        <v>620</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1395,7 +1520,7 @@
       </c>
       <c r="B25" s="6">
         <f>B17/B24</f>
-        <v>31.888888888888889</v>
+        <v>32.417741935483868</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1404,7 +1529,7 @@
       </c>
       <c r="B26" s="6">
         <f>B19/B15</f>
-        <v>0.18826657489505955</v>
+        <v>0.25536935177819819</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1413,7 +1538,7 @@
       </c>
       <c r="B27" s="6">
         <f>B14/B16</f>
-        <v>0.31763468897091196</v>
+        <v>0.26976376832218585</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -1421,8 +1546,8 @@
         <v>27</v>
       </c>
       <c r="B28" s="6">
-        <f>[1]R4R!E26</f>
-        <v>1100000</v>
+        <f>[1]R4R!M26</f>
+        <v>2209809.9493262982</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1430,8 +1555,8 @@
         <v>28</v>
       </c>
       <c r="B29" s="6">
-        <f>[1]R4R!E37</f>
-        <v>167716386.99774998</v>
+        <f>[1]R4R!M37</f>
+        <v>126474582.04596475</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -1439,8 +1564,8 @@
         <v>29</v>
       </c>
       <c r="B30" s="6">
-        <f>[1]R4R!E39</f>
-        <v>1915808.6847999992</v>
+        <f>[1]R4R!M39</f>
+        <v>1696355.7778052683</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1448,8 +1573,8 @@
         <v>50</v>
       </c>
       <c r="B31" s="6">
-        <f>[1]R4R!E40</f>
-        <v>4414079</v>
+        <f>[1]R4R!M40</f>
+        <v>765180.12408676615</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1457,7 +1582,7 @@
         <v>51</v>
       </c>
       <c r="B32" s="6">
-        <f>[1]R4R!E42</f>
+        <f>[1]R4R!M42</f>
         <v>0</v>
       </c>
     </row>
@@ -1466,7 +1591,7 @@
         <v>52</v>
       </c>
       <c r="B33" s="6">
-        <f>[1]R4R!E43</f>
+        <f>[1]R4R!M43</f>
         <v>0</v>
       </c>
     </row>
@@ -1475,8 +1600,8 @@
         <v>53</v>
       </c>
       <c r="B34" s="6">
-        <f>[1]R4R!E44</f>
-        <v>8475964.5531971008</v>
+        <f>[1]R4R!M44</f>
+        <v>7958639.9526595371</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1484,8 +1609,8 @@
         <v>30</v>
       </c>
       <c r="B35" s="6">
-        <f>[1]R4R!E45</f>
-        <v>8992347.2480222024</v>
+        <f>[1]R4R!M45</f>
+        <v>4685708.039493002</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1493,8 +1618,8 @@
         <v>31</v>
       </c>
       <c r="B36" s="6">
-        <f>[1]R4R!E46</f>
-        <v>32274693.513980698</v>
+        <f>[1]R4R!M46</f>
+        <v>27584187.476333722</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1502,8 +1627,8 @@
         <v>32</v>
       </c>
       <c r="B37" s="6">
-        <f>[1]R4R!E47</f>
-        <v>21488112.304190762</v>
+        <f>[1]R4R!M47</f>
+        <v>13930473.462220209</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1511,8 +1636,8 @@
         <v>33</v>
       </c>
       <c r="B38" s="6">
-        <f>[1]R4R!E48</f>
-        <v>6543614.858957001</v>
+        <f>[1]R4R!M48</f>
+        <v>3051304.4601880657</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1520,8 +1645,8 @@
         <v>35</v>
       </c>
       <c r="B39" s="6">
-        <f>[1]R4R!E49</f>
-        <v>3846666.5490708007</v>
+        <f>[1]R4R!M49</f>
+        <v>1725842.7947463281</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1529,8 +1654,8 @@
         <v>34</v>
       </c>
       <c r="B40" s="6">
-        <f>[1]R4R!E50</f>
-        <v>26541918.295966305</v>
+        <f>[1]R4R!M50</f>
+        <v>16924122.340030454</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1538,8 +1663,8 @@
         <v>36</v>
       </c>
       <c r="B41" s="6">
-        <f>[1]R4R!E52</f>
-        <v>1485160</v>
+        <f>[1]R4R!M52</f>
+        <v>1450919.5928848851</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -1547,7 +1672,8 @@
         <v>54</v>
       </c>
       <c r="B42" s="6">
-        <v>0</v>
+        <f>[1]R4R!M53</f>
+        <v>1525039.6573558222</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1555,8 +1681,8 @@
         <v>37</v>
       </c>
       <c r="B43" s="6">
-        <f>[1]R4R!E54</f>
-        <v>17174560.004198376</v>
+        <f>[1]R4R!M54</f>
+        <v>11478928.094861932</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -1564,8 +1690,8 @@
         <v>38</v>
       </c>
       <c r="B44" s="6">
-        <f>[1]R4R!E55</f>
-        <v>7153414.9939294979</v>
+        <f>[1]R4R!M55</f>
+        <v>6017422.8093521548</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -1573,8 +1699,8 @@
         <v>39</v>
       </c>
       <c r="B45" s="6">
-        <f>[1]R4R!E56</f>
-        <v>0</v>
+        <f>[1]R4R!M56</f>
+        <v>35515.288902255757</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -1582,8 +1708,8 @@
         <v>40</v>
       </c>
       <c r="B46" s="6">
-        <f>[1]R4R!E57</f>
-        <v>10494992.387217235</v>
+        <f>[1]R4R!M57</f>
+        <v>10454941.525389537</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1591,8 +1717,8 @@
         <v>41</v>
       </c>
       <c r="B47" s="6">
-        <f>[1]R4R!E58</f>
-        <v>8154123.2635999983</v>
+        <f>[1]R4R!M58</f>
+        <v>5951138.570044524</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -1600,8 +1726,8 @@
         <v>42</v>
       </c>
       <c r="B48" s="6">
-        <f>[1]R4R!E59</f>
-        <v>1560231.9930200002</v>
+        <f>[1]R4R!M59</f>
+        <v>884136.18510875478</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -1609,17 +1735,17 @@
         <v>43</v>
       </c>
       <c r="B49" s="6">
-        <f>[1]R4R!E60</f>
-        <v>233553</v>
+        <f>[1]R4R!M60</f>
+        <v>700230.30960916413</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B50" s="6">
-        <f>[1]R4R!E61</f>
-        <v>990810</v>
+        <f>[1]R4R!M61</f>
+        <v>178623.43460676802</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1627,8 +1753,8 @@
         <v>44</v>
       </c>
       <c r="B51" s="6">
-        <f>[1]R4R!E62</f>
-        <v>1921850.3476</v>
+        <f>[1]R4R!M62</f>
+        <v>651387.58731839038</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -1636,8 +1762,8 @@
         <v>45</v>
       </c>
       <c r="B52" s="6">
-        <f>[1]R4R!E63</f>
-        <v>308215</v>
+        <f>[1]R4R!M63</f>
+        <v>6022436.9343661135</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -1645,8 +1771,8 @@
         <v>46</v>
       </c>
       <c r="B53" s="6">
-        <f>[1]R4R!E64</f>
-        <v>0</v>
+        <f>[1]R4R!M64</f>
+        <v>983112.62860110216</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -1654,13 +1780,13 @@
         <v>47</v>
       </c>
       <c r="B54" s="6">
-        <f>[1]R4R!E65</f>
-        <v>3746271</v>
+        <f>[1]R4R!M65</f>
+        <v>1818935</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{899AD2C1-9A2D-48EE-90D5-D40BF0FD5974}"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{BA930769-1EFD-4F38-89CA-239472D8C702}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
price index page development
</commit_message>
<xml_diff>
--- a/public/dataTable.xlsx
+++ b/public/dataTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kotawski\Coding\estimationCenter\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/SATECHI/Programowanie/MyIdeas/estimation_center/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{572B8C6E-53A5-4AF6-B28D-2DCDD2DE4323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF19116-98FF-7A42-8A92-FE59A52D5A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F53F1143-5114-4282-8AF3-5DBDBA634C13}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{F53F1143-5114-4282-8AF3-5DBDBA634C13}"/>
   </bookViews>
   <sheets>
     <sheet name="EC" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="62">
   <si>
     <t>Nazwa</t>
   </si>
@@ -218,10 +218,13 @@
     <t>liczba kondygnacji nadziemnych</t>
   </si>
   <si>
-    <t>Wycena</t>
-  </si>
-  <si>
-    <t>Górczewska E4</t>
+    <t>Kraków</t>
+  </si>
+  <si>
+    <t>Jana Pawła</t>
+  </si>
+  <si>
+    <t>Kontraktacja</t>
   </si>
 </sst>
 </file>
@@ -229,7 +232,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -293,7 +296,7 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -304,14 +307,14 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Dziesiętny" xfId="2" builtinId="3"/>
@@ -338,233 +341,547 @@
       <xxl21:absoluteUrl r:id="rId2"/>
     </xxl21:alternateUrls>
     <sheetNames>
-      <sheetName val="Kody I"/>
-      <sheetName val="Powierzchnie"/>
-      <sheetName val="sieci cz.2"/>
-      <sheetName val="sieci"/>
-      <sheetName val="EC"/>
+      <sheetName val="Dmowskiego - Etap 2 Szczegóły"/>
+      <sheetName val="Dmowskiego - Etap 1 Szczegóły"/>
+      <sheetName val="Bardzka - wycinki"/>
+      <sheetName val="Bardzka - ektryczna"/>
+      <sheetName val="Bardzka - PORR GW"/>
+      <sheetName val="Bardzka  - CONTRACT SIGNEDv2"/>
+      <sheetName val="Bardzka  - CONTRACT SIGNED"/>
+      <sheetName val="Pohoskiego - kody I"/>
+      <sheetName val="Pohoskiego - contract signedv2"/>
+      <sheetName val="Pohoskiego - contract signed"/>
+      <sheetName val="Pohoskiego - zabezpieczenie wyk"/>
+      <sheetName val="Pohoskiego SS"/>
+      <sheetName val="Pohoskiego - windy"/>
+      <sheetName val="Pohoskiego - przylacza2"/>
+      <sheetName val="Pohoskiego - przylacza"/>
+      <sheetName val="Pohoskiego okna"/>
+      <sheetName val="Pohoskiego - drzwi"/>
+      <sheetName val="Pohoskiego - portale"/>
+      <sheetName val="Pohoskiego okna - an1"/>
+      <sheetName val="Pohoskiego - elektryka"/>
+      <sheetName val="Pohoskiego - instalacje sanitar"/>
+      <sheetName val="Pohoskiego - i sanitarne 2"/>
+      <sheetName val="Pohoskiego - elektryka an1"/>
+      <sheetName val="Pohoskiego - wezel"/>
+      <sheetName val="Pohoskiego - pzt"/>
+      <sheetName val="Pohoskiego roboty wykończeniowe"/>
+      <sheetName val="Romanowicza zabezpieczenie"/>
+      <sheetName val="Romanowicza - Express SS"/>
+      <sheetName val="Romanowicza - windy"/>
+      <sheetName val="Romanowicza - Express an1"/>
+      <sheetName val="Romanowicza - domofony"/>
+      <sheetName val="Romanowicza - MGBuilding"/>
+      <sheetName val="Romanowicza - MGBuilding2"/>
+      <sheetName val="Romanowicza - wykopy"/>
+      <sheetName val="Romanowicza Express an 3"/>
+      <sheetName val="Dmowskiego - Etap 1 Kody I"/>
+      <sheetName val="Dmowskiego - Etap 2 Kody I"/>
+      <sheetName val="Jana Pawła- KODY I "/>
+      <sheetName val="Jana Pawła - windy"/>
+      <sheetName val="Stocznia - SS"/>
+      <sheetName val="Stocznia - ściany szczelin A2"/>
+      <sheetName val="Stocznia - windy"/>
+      <sheetName val="Stocznia - GW"/>
+      <sheetName val="Stocznia badania archeologiczne"/>
+      <sheetName val="Stocznia - roboty ziemne"/>
+      <sheetName val="Stocznia - domofony"/>
+      <sheetName val="Stocznia - ściany szczeli A1"/>
+      <sheetName val="Stocznia - windy a1"/>
+      <sheetName val="Stocznia - przylacza"/>
+      <sheetName val="Stocznia Remediacja A1"/>
+      <sheetName val="Stocznia Remediacja"/>
+      <sheetName val="Stocznia - ogrodzenie"/>
+      <sheetName val="Stocznia - contract signedv2"/>
+      <sheetName val="Stocznia - contract signed"/>
+      <sheetName val="Romanowicza - contract signedv2"/>
+      <sheetName val="Romanowicza - contract signed"/>
+      <sheetName val="Stocznia - Keller"/>
+      <sheetName val="Brnenska - zasilanie placu budo"/>
+      <sheetName val="Brnenska - zabezpieczenia wykop"/>
+      <sheetName val="Brnenska adm an3"/>
+      <sheetName val="Brnenska adm an2"/>
+      <sheetName val="Brnenska adm an1"/>
+      <sheetName val="Brnenska adm"/>
+      <sheetName val="Brnenska kobi an1"/>
+      <sheetName val="Brnenska kobi"/>
+      <sheetName val="Brnenska wer dom an 2"/>
+      <sheetName val="Brnenska wer dom an 1"/>
+      <sheetName val="Brnenska wer dom"/>
+      <sheetName val="Brnenska szajowski an1"/>
+      <sheetName val="Brnenska szajowski"/>
+      <sheetName val="Brnenska SS"/>
+      <sheetName val="Brneńska przyłącza 4"/>
+      <sheetName val="Brneńska przyłącza"/>
+      <sheetName val="Brneńska przyłącza2"/>
+      <sheetName val="Brnenska - windy"/>
+      <sheetName val="Brneńska okna"/>
+      <sheetName val="Brneńska - sanitarne2"/>
+      <sheetName val="Brneńska - elektryka2"/>
+      <sheetName val="Brneńska - elew"/>
+      <sheetName val="Brneńska - wyk2"/>
+      <sheetName val="Brnenska - drzwi stalowe"/>
+      <sheetName val="Brnenska - witryny2"/>
+      <sheetName val="Brnenska - zabydowy meblowe2"/>
+      <sheetName val="Brneńska - bramy"/>
+      <sheetName val="Brneńska - drzwi2"/>
+      <sheetName val="Brneńska portale 2"/>
+      <sheetName val="Brneńska - żywica"/>
+      <sheetName val="Brneńska - domofony"/>
+      <sheetName val="Brneńska - droga"/>
+      <sheetName val="Brneńska - balustrady"/>
+      <sheetName val="Brneńska - podnosnik"/>
+      <sheetName val="Brneńska - wyk 3"/>
+      <sheetName val="Brneńska - elektryka"/>
+      <sheetName val="Brneńska - sanitarne3"/>
+      <sheetName val="Brneńska - wyk"/>
+      <sheetName val="Brneńska przyłącza3"/>
+      <sheetName val="Brneńska - drogaa"/>
+      <sheetName val="Brnenska -dfa"/>
+      <sheetName val="Brnenska - witryny"/>
+      <sheetName val="Brneńska portale"/>
+      <sheetName val="Brneńska - drzwi"/>
+      <sheetName val="Brnenska - zabydowy meblowe"/>
+      <sheetName val="Brneńska SS"/>
+      <sheetName val="Brneńska skrzynki na listy"/>
+      <sheetName val="Brneńska - master key"/>
+      <sheetName val="Brneńska - sanitarne"/>
+      <sheetName val="Brneńska siw"/>
+      <sheetName val="Brnenska - mur oporowy2"/>
+      <sheetName val="Brneńska - mur oporowy"/>
+      <sheetName val="Brneńska S0"/>
+      <sheetName val="Brnenska - geoprojekt"/>
+      <sheetName val="Jana Pawła - TES (4)"/>
+      <sheetName val="Jana Pawła - Oferta stan zero"/>
+      <sheetName val="Jana Pawła - Oferta nadziemie"/>
+      <sheetName val="Jana Pawła - deweloperski (4)"/>
+      <sheetName val="Jana Pawła - Drogi i Zieleń"/>
+      <sheetName val="Jana Pawła - Instalacje san"/>
+      <sheetName val="Jana Pawła - Inst.elektr."/>
+      <sheetName val="Zielony Politechnika Kody I"/>
+      <sheetName val="Zielony Zatoka Kody I"/>
+      <sheetName val="Zielony Trojkąt - rozbiorki"/>
+      <sheetName val="Zielony Trojkąt - windy2"/>
+      <sheetName val="Zielony Trojkąt - SS"/>
+      <sheetName val="Zielony Trojkąt - SS3"/>
+      <sheetName val="Zielony Trojkąt - SS2"/>
+      <sheetName val="Zielony Trojkąt - windy"/>
+      <sheetName val="Zielony Trojkąt - okna"/>
+      <sheetName val="Zielony Trojkąt - zasilanie pla"/>
+      <sheetName val="Zielony Trojkąt - przyl dla bud"/>
+      <sheetName val="Zielony Trojkąt - remediacja"/>
+      <sheetName val="Zielony Trojkąt - mury dzialowe"/>
+      <sheetName val="Zielony Trojkąt - mury"/>
+      <sheetName val="Zielony Trojkąt - sanitarne"/>
+      <sheetName val="Zielony Trojkat - budget"/>
+      <sheetName val="Curtis - Kody I"/>
+      <sheetName val="Opaczewska - Kody I"/>
+      <sheetName val="Brnenska - wyk2"/>
+      <sheetName val="Brnenska - wyk"/>
+      <sheetName val="Brnenska - contract signedv2"/>
+      <sheetName val="Brnenska - contract signed"/>
+      <sheetName val="R4R"/>
+      <sheetName val="Wykończenie budowlane"/>
+      <sheetName val="Stan surowy"/>
+      <sheetName val="EC - ROMANOWICZA"/>
+      <sheetName val="EC - STOCZNIA"/>
+      <sheetName val="EC - BRNEŃSKA"/>
+      <sheetName val="EC - POHOSKIEGO"/>
+      <sheetName val="EC - BARDZKA"/>
+      <sheetName val="EC - JANA PAWŁA"/>
+      <sheetName val="Opaczewska - keller"/>
+      <sheetName val="Bardzka - Kody I"/>
+      <sheetName val="udział SS do N03 - umowy"/>
+      <sheetName val="udział SS do N03 - wyceny"/>
+      <sheetName val="Park zachod budget in progress"/>
+      <sheetName val="Jaworska budget in progress"/>
+      <sheetName val="Kilińskiego budget in progress"/>
+      <sheetName val="Park Zachodni - umowy"/>
+      <sheetName val="Kilińskiego - umowy"/>
+      <sheetName val="Jaworska 2 - umowy"/>
+      <sheetName val="Windy zakupy centralne"/>
+      <sheetName val="Zielony T - Budmar"/>
+      <sheetName val="Stocznia - Promonte"/>
+      <sheetName val="Jana Pawła - Expres"/>
+      <sheetName val="Pohoskiego PRIŻ"/>
+      <sheetName val="Pohoskiego CONSTEEL"/>
+      <sheetName val="Brneńska ERBUD"/>
+      <sheetName val="Brneńska WIPEN"/>
+      <sheetName val="Brneńska GGTS"/>
+      <sheetName val="Romanowicza Aarsleff"/>
+      <sheetName val="Romanowicza Expres"/>
+      <sheetName val="Porównanie - WYCENY"/>
+      <sheetName val="Zielony T Politechnika Kody I"/>
+      <sheetName val="Zielony T Zatoka Kody I"/>
+      <sheetName val="Dmowskiego Etap 2 Kody I"/>
+      <sheetName val="Dmowskiego Etap 1 Kody I"/>
+      <sheetName val="Dmowskiego E1 + E2 Wycena szac"/>
+      <sheetName val="Jana Pawła - KODY I"/>
+      <sheetName val="Jana Pawła - Szczegóły"/>
+      <sheetName val="Pohoskiego - Szczegóły"/>
+      <sheetName val="Brneńska - Kody I"/>
+      <sheetName val="Brneńska - Szczegóły"/>
+      <sheetName val="Stocznia - Kody I"/>
+      <sheetName val="Romanowicza - Szczegóły"/>
+      <sheetName val="Romanowicza - Kody I"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="10">
-          <cell r="D10">
-            <v>5375</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="D11">
-            <v>1910</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="D12">
-            <v>555.79999999999995</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="D13">
-            <v>2458</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="D15">
-            <v>2417</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="D16">
-            <v>73</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="D17">
-            <v>7.8000000000001819</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="D18">
-            <v>9573.7000000000007</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="D19">
-            <v>1814.5</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="D20">
-            <v>7759.2</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="D21">
-            <v>6186</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="D23">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="D24">
-            <v>6186</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="D31">
-            <v>307</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="D35">
-            <v>60</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="D37">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="F41">
-            <v>97910</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="E54">
-            <v>6286.7566753109741</v>
-          </cell>
-          <cell r="F54">
-            <v>38889876.793473683</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="F55">
-            <v>839730.81040000007</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="F63">
-            <v>4428504.3724000007</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="F64">
-            <v>2057640</v>
-          </cell>
-        </row>
-        <row r="86">
-          <cell r="F86">
-            <v>7660528.7999999998</v>
-          </cell>
-        </row>
-        <row r="103">
-          <cell r="F103">
-            <v>4158826.816000001</v>
-          </cell>
-        </row>
-        <row r="136">
-          <cell r="D136">
-            <v>6232.9544000000014</v>
-          </cell>
-        </row>
-        <row r="137">
-          <cell r="F137">
-            <v>2065724</v>
-          </cell>
-        </row>
-        <row r="152">
-          <cell r="F152">
-            <v>725800</v>
-          </cell>
-        </row>
-        <row r="164">
-          <cell r="F164">
-            <v>5333664</v>
-          </cell>
-        </row>
-        <row r="194">
-          <cell r="F194">
-            <v>450000</v>
-          </cell>
-        </row>
-        <row r="201">
-          <cell r="F201">
-            <v>3276142.92</v>
-          </cell>
-        </row>
-        <row r="217">
-          <cell r="F217">
-            <v>1274055.5800000003</v>
-          </cell>
-        </row>
-        <row r="230">
-          <cell r="F230">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="237">
-          <cell r="F237">
-            <v>2189611.3200000003</v>
-          </cell>
-        </row>
-        <row r="251">
-          <cell r="F251">
-            <v>1459740.8800000004</v>
-          </cell>
-        </row>
-        <row r="288">
-          <cell r="F288">
-            <v>607080</v>
-          </cell>
-        </row>
-        <row r="302">
-          <cell r="F302">
-            <v>189605</v>
-          </cell>
-        </row>
-        <row r="314">
-          <cell r="F314">
-            <v>268800</v>
-          </cell>
-        </row>
-        <row r="324">
-          <cell r="F324">
-            <v>1997568.4550000001</v>
-          </cell>
-        </row>
-        <row r="345">
-          <cell r="F345">
-            <v>20000</v>
-          </cell>
-        </row>
-        <row r="351">
-          <cell r="F351">
-            <v>1771285.8396736842</v>
-          </cell>
-        </row>
-        <row r="366">
-          <cell r="F366">
-            <v>173208</v>
-          </cell>
-        </row>
-        <row r="377">
-          <cell r="F377">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1">
-        <row r="12">
-          <cell r="E12">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
       <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30"/>
+      <sheetData sheetId="31"/>
+      <sheetData sheetId="32"/>
+      <sheetData sheetId="33"/>
+      <sheetData sheetId="34"/>
+      <sheetData sheetId="35"/>
+      <sheetData sheetId="36"/>
+      <sheetData sheetId="37"/>
+      <sheetData sheetId="38"/>
+      <sheetData sheetId="39"/>
+      <sheetData sheetId="40"/>
+      <sheetData sheetId="41"/>
+      <sheetData sheetId="42"/>
+      <sheetData sheetId="43"/>
+      <sheetData sheetId="44"/>
+      <sheetData sheetId="45"/>
+      <sheetData sheetId="46"/>
+      <sheetData sheetId="47"/>
+      <sheetData sheetId="48"/>
+      <sheetData sheetId="49"/>
+      <sheetData sheetId="50"/>
+      <sheetData sheetId="51"/>
+      <sheetData sheetId="52"/>
+      <sheetData sheetId="53"/>
+      <sheetData sheetId="54"/>
+      <sheetData sheetId="55"/>
+      <sheetData sheetId="56"/>
+      <sheetData sheetId="57"/>
+      <sheetData sheetId="58"/>
+      <sheetData sheetId="59"/>
+      <sheetData sheetId="60"/>
+      <sheetData sheetId="61"/>
+      <sheetData sheetId="62"/>
+      <sheetData sheetId="63"/>
+      <sheetData sheetId="64"/>
+      <sheetData sheetId="65"/>
+      <sheetData sheetId="66"/>
+      <sheetData sheetId="67"/>
+      <sheetData sheetId="68"/>
+      <sheetData sheetId="69"/>
+      <sheetData sheetId="70"/>
+      <sheetData sheetId="71"/>
+      <sheetData sheetId="72"/>
+      <sheetData sheetId="73"/>
+      <sheetData sheetId="74"/>
+      <sheetData sheetId="75"/>
+      <sheetData sheetId="76"/>
+      <sheetData sheetId="77"/>
+      <sheetData sheetId="78"/>
+      <sheetData sheetId="79"/>
+      <sheetData sheetId="80"/>
+      <sheetData sheetId="81"/>
+      <sheetData sheetId="82"/>
+      <sheetData sheetId="83"/>
+      <sheetData sheetId="84"/>
+      <sheetData sheetId="85"/>
+      <sheetData sheetId="86"/>
+      <sheetData sheetId="87"/>
+      <sheetData sheetId="88"/>
+      <sheetData sheetId="89"/>
+      <sheetData sheetId="90"/>
+      <sheetData sheetId="91"/>
+      <sheetData sheetId="92"/>
+      <sheetData sheetId="93"/>
+      <sheetData sheetId="94"/>
+      <sheetData sheetId="95"/>
+      <sheetData sheetId="96"/>
+      <sheetData sheetId="97"/>
+      <sheetData sheetId="98"/>
+      <sheetData sheetId="99"/>
+      <sheetData sheetId="100"/>
+      <sheetData sheetId="101"/>
+      <sheetData sheetId="102"/>
+      <sheetData sheetId="103"/>
+      <sheetData sheetId="104"/>
+      <sheetData sheetId="105"/>
+      <sheetData sheetId="106"/>
+      <sheetData sheetId="107"/>
+      <sheetData sheetId="108"/>
+      <sheetData sheetId="109"/>
+      <sheetData sheetId="110"/>
+      <sheetData sheetId="111"/>
+      <sheetData sheetId="112"/>
+      <sheetData sheetId="113"/>
+      <sheetData sheetId="114"/>
+      <sheetData sheetId="115"/>
+      <sheetData sheetId="116"/>
+      <sheetData sheetId="117"/>
+      <sheetData sheetId="118"/>
+      <sheetData sheetId="119"/>
+      <sheetData sheetId="120"/>
+      <sheetData sheetId="121"/>
+      <sheetData sheetId="122"/>
+      <sheetData sheetId="123"/>
+      <sheetData sheetId="124"/>
+      <sheetData sheetId="125"/>
+      <sheetData sheetId="126"/>
+      <sheetData sheetId="127"/>
+      <sheetData sheetId="128"/>
+      <sheetData sheetId="129"/>
+      <sheetData sheetId="130"/>
+      <sheetData sheetId="131"/>
+      <sheetData sheetId="132"/>
+      <sheetData sheetId="133"/>
+      <sheetData sheetId="134"/>
+      <sheetData sheetId="135"/>
+      <sheetData sheetId="136"/>
+      <sheetData sheetId="137"/>
+      <sheetData sheetId="138"/>
+      <sheetData sheetId="139"/>
+      <sheetData sheetId="140">
+        <row r="4">
+          <cell r="O4">
+            <v>3424</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="O5">
+            <v>709.75</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="O6">
+            <v>815</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="O12">
+            <v>815</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="O13">
+            <v>10439.269999999999</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="O14">
+            <v>8179.3799999999992</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="O15">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="O16">
+            <v>8179.3799999999992</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="O21">
+            <v>27</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="O22">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="O23">
+            <v>283</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="O32">
+            <v>60000</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="O43">
+            <v>49500425.507282011</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="O45">
+            <v>360110.00799999997</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="O46">
+            <v>129600</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="O50">
+            <v>1680710.58038264</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="O51">
+            <v>1310570.0434726416</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="O52">
+            <v>10564070.756622612</v>
+          </cell>
+        </row>
+        <row r="53">
+          <cell r="O53">
+            <v>5445201.6796182012</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="O54">
+            <v>1245665.1108137181</v>
+          </cell>
+        </row>
+        <row r="55">
+          <cell r="O55">
+            <v>238630.32105175586</v>
+          </cell>
+        </row>
+        <row r="56">
+          <cell r="O56">
+            <v>9295885.167720465</v>
+          </cell>
+        </row>
+        <row r="58">
+          <cell r="O58">
+            <v>871310.00000000012</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="O60">
+            <v>6412317.7369045932</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="O61">
+            <v>2117531.2459094571</v>
+          </cell>
+        </row>
+        <row r="62">
+          <cell r="O62">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="O63">
+            <v>3434855.2912000008</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="O64">
+            <v>2990955.4448000002</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="O65">
+            <v>529564.62078593671</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="O66">
+            <v>73371.5</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="O67">
+            <v>84674.5</v>
+          </cell>
+        </row>
+        <row r="68">
+          <cell r="O68">
+            <v>837680.5</v>
+          </cell>
+        </row>
+        <row r="69">
+          <cell r="O69">
+            <v>1622950</v>
+          </cell>
+        </row>
+        <row r="70">
+          <cell r="O70">
+            <v>254771</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="141"/>
+      <sheetData sheetId="142"/>
+      <sheetData sheetId="143"/>
+      <sheetData sheetId="144"/>
+      <sheetData sheetId="145"/>
+      <sheetData sheetId="146"/>
+      <sheetData sheetId="147"/>
+      <sheetData sheetId="148"/>
+      <sheetData sheetId="149"/>
+      <sheetData sheetId="150"/>
+      <sheetData sheetId="151"/>
+      <sheetData sheetId="152"/>
+      <sheetData sheetId="153"/>
+      <sheetData sheetId="154"/>
+      <sheetData sheetId="155"/>
+      <sheetData sheetId="156"/>
+      <sheetData sheetId="157"/>
+      <sheetData sheetId="158"/>
+      <sheetData sheetId="159"/>
+      <sheetData sheetId="160"/>
+      <sheetData sheetId="161"/>
+      <sheetData sheetId="162"/>
+      <sheetData sheetId="163"/>
+      <sheetData sheetId="164"/>
+      <sheetData sheetId="165"/>
+      <sheetData sheetId="166"/>
+      <sheetData sheetId="167"/>
+      <sheetData sheetId="168"/>
+      <sheetData sheetId="169"/>
+      <sheetData sheetId="170"/>
+      <sheetData sheetId="171"/>
+      <sheetData sheetId="172"/>
+      <sheetData sheetId="173"/>
+      <sheetData sheetId="174"/>
+      <sheetData sheetId="175"/>
+      <sheetData sheetId="176"/>
+      <sheetData sheetId="177"/>
+      <sheetData sheetId="178"/>
+      <sheetData sheetId="179"/>
+      <sheetData sheetId="180"/>
+      <sheetData sheetId="181"/>
+      <sheetData sheetId="182"/>
+      <sheetData sheetId="183"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -893,13 +1210,13 @@
       <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -907,15 +1224,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="96" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -923,475 +1240,470 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="4">
-        <f>'[1]Kody I'!E54</f>
-        <v>6286.7566753109741</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <f>[1]R4R!O43/[1]R4R!O16</f>
+        <v>6051.855459372473</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="6">
-        <f>'[1]Kody I'!D10</f>
-        <v>5375</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <f>[1]R4R!O4</f>
+        <v>3424</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>54</v>
       </c>
       <c r="B7" s="6">
-        <f>'[1]Kody I'!D13</f>
-        <v>2458</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <f>[1]R4R!O5</f>
+        <v>709.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>55</v>
       </c>
       <c r="B8" s="6">
-        <f>'[1]Kody I'!D11</f>
-        <v>1910</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <f>[1]R4R!O6</f>
+        <v>815</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B9" s="6">
-        <f>'[1]Kody I'!D12</f>
-        <v>555.79999999999995</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>709.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="6">
         <f>B6-B7</f>
-        <v>2917</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2714.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="6">
-        <f>'[1]Kody I'!D15+'[1]Kody I'!D16+'[1]Kody I'!D17</f>
-        <v>2497.8000000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1587</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="6">
-        <f>'[1]Kody I'!D136</f>
-        <v>6232.9544000000014</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8992.8556599999993</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="6">
-        <f>'[1]Kody I'!D18</f>
-        <v>9573.7000000000007</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <f>B14+B15</f>
+        <v>11254.269999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="6">
-        <f>'[1]Kody I'!D19</f>
-        <v>1814.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <f>[1]R4R!O12</f>
+        <v>815</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="6">
-        <f>'[1]Kody I'!D20</f>
-        <v>7759.2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <f>[1]R4R!O13</f>
+        <v>10439.269999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="6">
-        <f>'[1]Kody I'!D21</f>
-        <v>6186</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <f>B17+B18</f>
+        <v>8179.3799999999992</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="6">
-        <f>'[1]Kody I'!D24</f>
-        <v>6186</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <f>[1]R4R!O14</f>
+        <v>8179.3799999999992</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="6">
-        <f>'[1]Kody I'!D23</f>
+        <f>[1]R4R!O15</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="6">
         <f>B15-B17-B18</f>
-        <v>1573.1999999999998</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2259.8899999999994</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="6">
-        <f>[1]Powierzchnie!E12</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>57</v>
       </c>
       <c r="B21" s="6">
-        <f>1</f>
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B22" s="6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B23" s="6">
-        <f>'[1]Kody I'!D35</f>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <f>[1]R4R!O21</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B24" s="6">
-        <f>'[1]Kody I'!D37</f>
+        <f>[1]R4R!O22</f>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B25" s="6">
-        <f>'[1]Kody I'!D31</f>
-        <v>307</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <f>[1]R4R!O23</f>
+        <v>283</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B26" s="6">
         <f>B17/B25</f>
-        <v>20.149837133550488</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>28.90240282685512</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B27" s="6">
         <f>B19/B15</f>
-        <v>0.20275286111970303</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.21647969637723707</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B28" s="6">
         <f>B14/B16</f>
-        <v>0.29332363401228578</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>9.964080407072419E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B29" s="6">
-        <f>'[1]Kody I'!F41</f>
-        <v>97910</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <f>[1]R4R!O32</f>
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B30" s="6">
-        <f>'[1]Kody I'!F54</f>
-        <v>38889876.793473683</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <f>[1]R4R!O43</f>
+        <v>49500425.507282011</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B31" s="6">
-        <f>'[1]Kody I'!F55-'[1]Kody I'!F61</f>
-        <v>839730.81040000007</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <f>[1]R4R!O45</f>
+        <v>360110.00799999997</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B32" s="6">
-        <f>'[1]Kody I'!F61</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <f>[1]R4R!O46</f>
+        <v>129600</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B33" s="6">
-        <f>'[1]Kody I'!F77</f>
+        <f>[1]R4R!O48</f>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B34" s="6">
-        <f>'[1]Kody I'!F74</f>
+        <f>[1]R4R!O49</f>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B35" s="6">
-        <f>'[1]Kody I'!F63-'[1]Kody I'!F64-'[1]Kody I'!F77-'[1]Kody I'!F74</f>
-        <v>2370864.3724000007</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+        <f>[1]R4R!O50</f>
+        <v>1680710.58038264</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B36" s="6">
-        <f>'[1]Kody I'!F64</f>
-        <v>2057640</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+        <f>[1]R4R!O51</f>
+        <v>1310570.0434726416</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B37" s="6">
-        <f>'[1]Kody I'!F86</f>
-        <v>7660528.7999999998</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <f>[1]R4R!O52</f>
+        <v>10564070.756622612</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B38" s="6">
-        <f>'[1]Kody I'!F103</f>
-        <v>4158826.816000001</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+        <f>[1]R4R!O53</f>
+        <v>5445201.6796182012</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B39" s="6">
-        <f>'[1]Kody I'!F137</f>
-        <v>2065724</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+        <f>[1]R4R!O54</f>
+        <v>1245665.1108137181</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B40" s="6">
-        <f>'[1]Kody I'!F152</f>
-        <v>725800</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+        <f>[1]R4R!O55</f>
+        <v>238630.32105175586</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B41" s="6">
-        <f>'[1]Kody I'!F164</f>
-        <v>5333664</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+        <f>[1]R4R!O56</f>
+        <v>9295885.167720465</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B42" s="6">
-        <f>'[1]Kody I'!F194-'[1]Kody I'!F199</f>
-        <v>450000</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+        <f>[1]R4R!O58</f>
+        <v>871310.00000000012</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B43" s="6">
-        <f>'[1]Kody I'!F199</f>
+        <f>[1]R4R!O59</f>
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B44" s="6">
-        <f>'[1]Kody I'!F201</f>
-        <v>3276142.92</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+        <f>[1]R4R!O60</f>
+        <v>6412317.7369045932</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B45" s="6">
-        <f>'[1]Kody I'!F217</f>
-        <v>1274055.5800000003</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+        <f>[1]R4R!O61</f>
+        <v>2117531.2459094571</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B46" s="6">
-        <f>'[1]Kody I'!F230</f>
+        <f>[1]R4R!O62</f>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B47" s="6">
-        <f>'[1]Kody I'!F237</f>
-        <v>2189611.3200000003</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+        <f>[1]R4R!O63</f>
+        <v>3434855.2912000008</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B48" s="6">
-        <f>'[1]Kody I'!F251</f>
-        <v>1459740.8800000004</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+        <f>[1]R4R!O64</f>
+        <v>2990955.4448000002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B49" s="6">
-        <f>'[1]Kody I'!F288+'[1]Kody I'!F345</f>
-        <v>627080</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+        <f>[1]R4R!O65</f>
+        <v>529564.62078593671</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B50" s="6">
-        <f>'[1]Kody I'!F302</f>
-        <v>189605</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+        <f>[1]R4R!O66</f>
+        <v>73371.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>56</v>
       </c>
       <c r="B51" s="6">
-        <f>'[1]Kody I'!F314</f>
-        <v>268800</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+        <f>[1]R4R!O67</f>
+        <v>84674.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B52" s="6">
-        <f>'[1]Kody I'!F324</f>
-        <v>1997568.4550000001</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+        <f>[1]R4R!O68</f>
+        <v>837680.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B53" s="6">
-        <f>'[1]Kody I'!F351</f>
-        <v>1771285.8396736842</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+        <f>[1]R4R!O69</f>
+        <v>1622950</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B54" s="6">
-        <f>'[1]Kody I'!F366</f>
-        <v>173208</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+        <f>[1]R4R!O70</f>
+        <v>254771</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B55" s="6">
-        <f>'[1]Kody I'!F377</f>
+        <f>[1]R4R!O71</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{8FA41D15-A840-4FE5-8A17-2C4BF5FC5F9D}"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{5B5ABE0B-4E15-BF4E-8004-CB4B9162EACA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1405,9 +1717,9 @@
       <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1424,7 +1736,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="208" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>

</xml_diff>